<commit_message>
Mise à jour de la burndown chart
</commit_message>
<xml_diff>
--- a/team/BurndownChart.xlsx
+++ b/team/BurndownChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26306"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\ULB\BA3\ulb-rhumblet\BA3\INFO-F307 - Génie logiciel et gestion de projets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brenn\IdeaProjects\2023-groupe-12\team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="349" documentId="8_{098DEF6D-6F1F-40CF-8599-A180A09D0F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2667EBC-609E-4575-9A13-95F668AD06E8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D75796C-532F-4F0C-99AA-AA39D982F300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="104">
   <si>
     <t>Estimation</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>HISTOIRE 13</t>
+  </si>
+  <si>
+    <t>Tâche 4 (Connexion, Utilisateur, validation)</t>
   </si>
 </sst>
 </file>
@@ -819,30 +822,30 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="cf1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -918,7 +921,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -986,16 +989,16 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4</c:v>
+                  <c:v>-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4</c:v>
+                  <c:v>-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-44</c:v>
+                  <c:v>-46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-44</c:v>
+                  <c:v>-46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2614,7 +2617,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1212754608"/>
@@ -2646,7 +2649,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1212753776"/>
@@ -2690,7 +2693,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -2747,16 +2750,16 @@
                   <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-481</c:v>
+                  <c:v>-483</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-846</c:v>
+                  <c:v>-848</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1531</c:v>
+                  <c:v>-1533</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2815,7 +2818,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1219476176"/>
@@ -2847,7 +2850,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1219475344"/>
@@ -2883,7 +2886,7 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2907,7 +2910,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -3160,7 +3163,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1121229456"/>
@@ -3192,7 +3195,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="951912112"/>
@@ -3228,7 +3231,7 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3252,7 +3255,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -3505,7 +3508,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1216119696"/>
@@ -3537,7 +3540,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1212759184"/>
@@ -3573,7 +3576,7 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3597,7 +3600,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -3850,7 +3853,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1222438416"/>
@@ -3882,7 +3885,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1222442160"/>
@@ -3918,7 +3921,7 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3942,7 +3945,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -4195,7 +4198,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1222435504"/>
@@ -4227,7 +4230,7 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1222438832"/>
@@ -4263,7 +4266,7 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4469,7 +4472,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4767,23 +4770,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="C2" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="7" width="11.85546875" customWidth="1"/>
+    <col min="1" max="7" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="14.45">
+    <row r="1" spans="2:7">
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="2:7" ht="14.45">
+    <row r="2" spans="2:7">
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -4800,7 +4803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="14.45">
+    <row r="3" spans="2:7">
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
@@ -4809,22 +4812,22 @@
       </c>
       <c r="D3" s="10">
         <f>C3-_xlfn.SINGLE(IT1H1)</f>
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="E3" s="11">
         <f>D3-_xlfn.SINGLE(IT2H1)</f>
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="F3" s="10">
         <f>E3-_xlfn.SINGLE(IT3H1)</f>
-        <v>-44</v>
+        <v>-46</v>
       </c>
       <c r="G3" s="12">
         <f>F3-_xlfn.SINGLE(IT4H1)</f>
-        <v>-44</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="14.45">
+        <v>-46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
@@ -4848,7 +4851,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="14.45">
+    <row r="5" spans="2:7">
       <c r="B5" s="13" t="s">
         <v>7</v>
       </c>
@@ -4872,7 +4875,7 @@
         <v>-36</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="14.45">
+    <row r="6" spans="2:7">
       <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
@@ -4896,7 +4899,7 @@
         <v>-52</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="14.45">
+    <row r="7" spans="2:7">
       <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
@@ -4920,7 +4923,7 @@
         <v>-93</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="14.45">
+    <row r="8" spans="2:7">
       <c r="B8" s="13" t="s">
         <v>10</v>
       </c>
@@ -4944,7 +4947,7 @@
         <v>-71</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="14.45">
+    <row r="9" spans="2:7">
       <c r="B9" s="13" t="s">
         <v>11</v>
       </c>
@@ -4968,7 +4971,7 @@
         <v>-112</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="14.45">
+    <row r="10" spans="2:7">
       <c r="B10" s="13" t="s">
         <v>12</v>
       </c>
@@ -4992,7 +4995,7 @@
         <v>-69</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="14.45">
+    <row r="11" spans="2:7">
       <c r="B11" s="13" t="s">
         <v>13</v>
       </c>
@@ -5016,7 +5019,7 @@
         <v>-110</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="14.45">
+    <row r="12" spans="2:7">
       <c r="B12" s="13" t="s">
         <v>14</v>
       </c>
@@ -5040,7 +5043,7 @@
         <v>-61</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="14.45">
+    <row r="13" spans="2:7">
       <c r="B13" s="13" t="s">
         <v>15</v>
       </c>
@@ -5064,7 +5067,7 @@
         <v>-110</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="14.45">
+    <row r="14" spans="2:7">
       <c r="B14" s="13" t="s">
         <v>16</v>
       </c>
@@ -5088,7 +5091,7 @@
         <v>-38</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="14.45">
+    <row r="15" spans="2:7">
       <c r="B15" s="18" t="s">
         <v>17</v>
       </c>
@@ -5096,23 +5099,23 @@
         <v>14</v>
       </c>
       <c r="D15" s="20">
-        <f>C15-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" ref="D15:D24" si="0">C15-_xlfn.SINGLE(IT1H13)</f>
         <v>14</v>
       </c>
       <c r="E15" s="21">
-        <f>D15-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" ref="E15:E24" si="1">D15-_xlfn.SINGLE(IT2H13)</f>
         <v>-26</v>
       </c>
       <c r="F15" s="20">
-        <f>E15-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" ref="F15:F24" si="2">E15-_xlfn.SINGLE(IT3H13)</f>
         <v>-26</v>
       </c>
       <c r="G15" s="22">
-        <f>F15-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" ref="G15:G24" si="3">F15-_xlfn.SINGLE(IT4H13)</f>
         <v>-66</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="15">
+    <row r="16" spans="2:7">
       <c r="B16" s="18" t="s">
         <v>18</v>
       </c>
@@ -5120,23 +5123,23 @@
         <v>4</v>
       </c>
       <c r="D16" s="20">
-        <f>C16-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E16" s="21">
-        <f>D16-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" si="1"/>
         <v>-36</v>
       </c>
       <c r="F16" s="20">
-        <f>E16-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" si="2"/>
         <v>-36</v>
       </c>
       <c r="G16" s="22">
-        <f>F16-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" si="3"/>
         <v>-76</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="15">
+    <row r="17" spans="2:7">
       <c r="B17" s="18" t="s">
         <v>19</v>
       </c>
@@ -5144,23 +5147,23 @@
         <v>6</v>
       </c>
       <c r="D17" s="20">
-        <f>C17-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E17" s="21">
-        <f>D17-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" si="1"/>
         <v>-34</v>
       </c>
       <c r="F17" s="20">
-        <f>E17-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" si="2"/>
         <v>-34</v>
       </c>
       <c r="G17" s="22">
-        <f>F17-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" si="3"/>
         <v>-74</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="15">
+    <row r="18" spans="2:7">
       <c r="B18" s="18" t="s">
         <v>20</v>
       </c>
@@ -5168,23 +5171,23 @@
         <v>4</v>
       </c>
       <c r="D18" s="20">
-        <f>C18-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E18" s="21">
-        <f>D18-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" si="1"/>
         <v>-36</v>
       </c>
       <c r="F18" s="20">
-        <f>E18-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" si="2"/>
         <v>-36</v>
       </c>
       <c r="G18" s="22">
-        <f>F18-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" si="3"/>
         <v>-76</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15">
+    <row r="19" spans="2:7">
       <c r="B19" s="18" t="s">
         <v>21</v>
       </c>
@@ -5192,23 +5195,23 @@
         <v>5</v>
       </c>
       <c r="D19" s="20">
-        <f>C19-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E19" s="21">
-        <f>D19-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" si="1"/>
         <v>-35</v>
       </c>
       <c r="F19" s="20">
-        <f>E19-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" si="2"/>
         <v>-35</v>
       </c>
       <c r="G19" s="22">
-        <f>F19-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" si="3"/>
         <v>-75</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="15">
+    <row r="20" spans="2:7">
       <c r="B20" s="18" t="s">
         <v>22</v>
       </c>
@@ -5216,23 +5219,23 @@
         <v>15</v>
       </c>
       <c r="D20" s="20">
-        <f>C20-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E20" s="21">
-        <f>D20-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" si="1"/>
         <v>-25</v>
       </c>
       <c r="F20" s="20">
-        <f>E20-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" si="2"/>
         <v>-25</v>
       </c>
       <c r="G20" s="22">
-        <f>F20-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" si="3"/>
         <v>-65</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="15">
+    <row r="21" spans="2:7">
       <c r="B21" s="18" t="s">
         <v>23</v>
       </c>
@@ -5240,23 +5243,23 @@
         <v>8</v>
       </c>
       <c r="D21" s="20">
-        <f>C21-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E21" s="21">
-        <f>D21-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" si="1"/>
         <v>-32</v>
       </c>
       <c r="F21" s="20">
-        <f>E21-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" si="2"/>
         <v>-32</v>
       </c>
       <c r="G21" s="22">
-        <f>F21-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" si="3"/>
         <v>-72</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15">
+    <row r="22" spans="2:7">
       <c r="B22" s="18" t="s">
         <v>24</v>
       </c>
@@ -5264,23 +5267,23 @@
         <v>10</v>
       </c>
       <c r="D22" s="20">
-        <f>C22-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E22" s="21">
-        <f>D22-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" si="1"/>
         <v>-30</v>
       </c>
       <c r="F22" s="20">
-        <f>E22-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" si="2"/>
         <v>-30</v>
       </c>
       <c r="G22" s="22">
-        <f>F22-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" si="3"/>
         <v>-70</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="15">
+    <row r="23" spans="2:7">
       <c r="B23" s="18" t="s">
         <v>25</v>
       </c>
@@ -5288,23 +5291,23 @@
         <v>4</v>
       </c>
       <c r="D23" s="20">
-        <f>C23-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E23" s="21">
-        <f>D23-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" si="1"/>
         <v>-36</v>
       </c>
       <c r="F23" s="20">
-        <f>E23-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" si="2"/>
         <v>-36</v>
       </c>
       <c r="G23" s="22">
-        <f>F23-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" si="3"/>
         <v>-76</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="15">
+    <row r="24" spans="2:7">
       <c r="B24" s="18" t="s">
         <v>26</v>
       </c>
@@ -5312,23 +5315,23 @@
         <v>14</v>
       </c>
       <c r="D24" s="20">
-        <f>C24-_xlfn.SINGLE(IT1H13)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E24" s="21">
-        <f>D24-_xlfn.SINGLE(IT2H13)</f>
+        <f t="shared" si="1"/>
         <v>-26</v>
       </c>
       <c r="F24" s="20">
-        <f>E24-_xlfn.SINGLE(IT3H13)</f>
+        <f t="shared" si="2"/>
         <v>-26</v>
       </c>
       <c r="G24" s="22">
-        <f>F24-_xlfn.SINGLE(IT4H13)</f>
+        <f t="shared" si="3"/>
         <v>-66</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="15">
+    <row r="25" spans="2:7">
       <c r="B25" s="41"/>
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
@@ -5336,7 +5339,7 @@
       <c r="F25" s="20"/>
       <c r="G25" s="22"/>
     </row>
-    <row r="26" spans="2:7" ht="14.45">
+    <row r="26" spans="2:7">
       <c r="C26" s="4" t="s">
         <v>0</v>
       </c>
@@ -5360,19 +5363,19 @@
       </c>
       <c r="D27" s="42">
         <f>SUM(D3:D24)</f>
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E27" s="42">
         <f>SUM(E3:E24)</f>
-        <v>-481</v>
+        <v>-483</v>
       </c>
       <c r="F27" s="42">
         <f>SUM(F3:F24)</f>
-        <v>-846</v>
+        <v>-848</v>
       </c>
       <c r="G27" s="42">
         <f>SUM(G3:G24)</f>
-        <v>-1531</v>
+        <v>-1533</v>
       </c>
     </row>
   </sheetData>
@@ -5387,77 +5390,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMI124"/>
+  <dimension ref="A1:AMI106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="23" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="15" style="23" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" style="23" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="23" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" style="23" customWidth="1"/>
-    <col min="8" max="259" width="14.85546875" style="23" customWidth="1"/>
-    <col min="260" max="260" width="13.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="55.44140625" style="23" customWidth="1"/>
+    <col min="4" max="5" width="17.44140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" style="23" customWidth="1"/>
+    <col min="8" max="259" width="14.88671875" style="23" customWidth="1"/>
+    <col min="260" max="260" width="13.6640625" style="23" customWidth="1"/>
     <col min="261" max="261" width="15" style="23" customWidth="1"/>
-    <col min="262" max="262" width="55.42578125" style="23" customWidth="1"/>
-    <col min="263" max="263" width="33.5703125" style="23" customWidth="1"/>
-    <col min="264" max="264" width="32.7109375" style="23" customWidth="1"/>
-    <col min="265" max="265" width="26.28515625" style="23" customWidth="1"/>
-    <col min="266" max="515" width="14.85546875" style="23" customWidth="1"/>
-    <col min="516" max="516" width="13.7109375" style="23" customWidth="1"/>
+    <col min="262" max="262" width="55.44140625" style="23" customWidth="1"/>
+    <col min="263" max="263" width="33.5546875" style="23" customWidth="1"/>
+    <col min="264" max="264" width="32.6640625" style="23" customWidth="1"/>
+    <col min="265" max="265" width="26.33203125" style="23" customWidth="1"/>
+    <col min="266" max="515" width="14.88671875" style="23" customWidth="1"/>
+    <col min="516" max="516" width="13.6640625" style="23" customWidth="1"/>
     <col min="517" max="517" width="15" style="23" customWidth="1"/>
-    <col min="518" max="518" width="55.42578125" style="23" customWidth="1"/>
-    <col min="519" max="519" width="33.5703125" style="23" customWidth="1"/>
-    <col min="520" max="520" width="32.7109375" style="23" customWidth="1"/>
-    <col min="521" max="521" width="26.28515625" style="23" customWidth="1"/>
-    <col min="522" max="771" width="14.85546875" style="23" customWidth="1"/>
-    <col min="772" max="772" width="13.7109375" style="23" customWidth="1"/>
+    <col min="518" max="518" width="55.44140625" style="23" customWidth="1"/>
+    <col min="519" max="519" width="33.5546875" style="23" customWidth="1"/>
+    <col min="520" max="520" width="32.6640625" style="23" customWidth="1"/>
+    <col min="521" max="521" width="26.33203125" style="23" customWidth="1"/>
+    <col min="522" max="771" width="14.88671875" style="23" customWidth="1"/>
+    <col min="772" max="772" width="13.6640625" style="23" customWidth="1"/>
     <col min="773" max="773" width="15" style="23" customWidth="1"/>
-    <col min="774" max="774" width="55.42578125" style="23" customWidth="1"/>
-    <col min="775" max="775" width="33.5703125" style="23" customWidth="1"/>
-    <col min="776" max="776" width="32.7109375" style="23" customWidth="1"/>
-    <col min="777" max="777" width="26.28515625" style="23" customWidth="1"/>
-    <col min="778" max="1023" width="14.85546875" style="23" customWidth="1"/>
+    <col min="774" max="774" width="55.44140625" style="23" customWidth="1"/>
+    <col min="775" max="775" width="33.5546875" style="23" customWidth="1"/>
+    <col min="776" max="776" width="32.6640625" style="23" customWidth="1"/>
+    <col min="777" max="777" width="26.33203125" style="23" customWidth="1"/>
+    <col min="778" max="1023" width="14.88671875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="14.45">
-      <c r="K1" s="45" t="s">
+    <row r="1" spans="1:22">
+      <c r="K1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:22" ht="20.25" customHeight="1">
       <c r="A2" s="25"/>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="K2" s="45" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="K2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45" t="s">
+      <c r="L2" s="46"/>
+      <c r="M2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45" t="s">
+      <c r="N2" s="46"/>
+      <c r="O2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45" t="s">
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="45"/>
+      <c r="R2" s="46"/>
       <c r="U2" s="43" t="s">
         <v>30</v>
       </c>
@@ -5479,10 +5482,10 @@
       <c r="G3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="45"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="24" t="s">
         <v>37</v>
       </c>
@@ -5536,7 +5539,7 @@
       <c r="J4" s="30">
         <v>0</v>
       </c>
-      <c r="K4" s="50">
+      <c r="K4" s="44">
         <f>$G$11*(1-1/$I$19*J4)</f>
         <v>6</v>
       </c>
@@ -5562,11 +5565,11 @@
         <v>35</v>
       </c>
       <c r="U4" s="23">
-        <f>K4+M4+O4+Q4</f>
+        <f t="shared" ref="U4:V8" si="0">K4+M4+O4+Q4</f>
         <v>96</v>
       </c>
       <c r="V4" s="23">
-        <f>L4+N4+P4+R4</f>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
     </row>
@@ -5593,7 +5596,7 @@
       <c r="J5" s="30">
         <v>1</v>
       </c>
-      <c r="K5" s="50">
+      <c r="K5" s="44">
         <f>$G$11*(1-1/$I$19*J5)</f>
         <v>5.5714285714285712</v>
       </c>
@@ -5619,11 +5622,11 @@
         <v>30</v>
       </c>
       <c r="U5" s="23">
-        <f>K5+M5+O5+Q5</f>
+        <f t="shared" si="0"/>
         <v>80.571428571428569</v>
       </c>
       <c r="V5" s="23">
-        <f>L5+N5+P5+R5</f>
+        <f t="shared" si="0"/>
         <v>123</v>
       </c>
     </row>
@@ -5649,7 +5652,7 @@
       <c r="J6" s="30">
         <v>2</v>
       </c>
-      <c r="K6" s="50">
+      <c r="K6" s="44">
         <f>$G$11*(1-1/$I$12*J6)</f>
         <v>5.9997332918453985</v>
       </c>
@@ -5675,21 +5678,27 @@
         <v>31</v>
       </c>
       <c r="U6" s="23">
-        <f>K6+M6+O6+Q6</f>
+        <f t="shared" si="0"/>
         <v>71.999733291845402</v>
       </c>
       <c r="V6" s="23">
-        <f>L6+N6+P6+R6</f>
+        <f t="shared" si="0"/>
         <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15" customHeight="1">
       <c r="C7" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
+        <v>103</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="28">
+        <v>2</v>
+      </c>
       <c r="G7" s="28"/>
       <c r="I7" s="29">
         <v>44988</v>
@@ -5697,7 +5706,7 @@
       <c r="J7" s="30">
         <v>3</v>
       </c>
-      <c r="K7" s="50">
+      <c r="K7" s="44">
         <f>$G$11*(1-1/$I$12*J7)</f>
         <v>5.9995999377680969</v>
       </c>
@@ -5723,11 +5732,11 @@
         <v>26</v>
       </c>
       <c r="U7" s="23">
-        <f>K7+M7+O7+Q7</f>
+        <f t="shared" si="0"/>
         <v>80.999599937768096</v>
       </c>
       <c r="V7" s="23">
-        <f>L7+N7+P7+R7</f>
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
     </row>
@@ -5745,7 +5754,7 @@
       <c r="J8" s="30">
         <v>4</v>
       </c>
-      <c r="K8" s="50">
+      <c r="K8" s="44">
         <f>$G$11*(1-1/$I$12*J8)</f>
         <v>5.9994665836907961</v>
       </c>
@@ -5771,11 +5780,11 @@
         <v>12</v>
       </c>
       <c r="U8" s="23">
-        <f>K8+M8+O8+Q8</f>
+        <f t="shared" si="0"/>
         <v>35.999466583690797</v>
       </c>
       <c r="V8" s="23">
-        <f>L8+N8+P8+R8</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
@@ -5877,14 +5886,14 @@
     </row>
     <row r="11" spans="1:22" ht="18" customHeight="1">
       <c r="A11" s="31"/>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="32">
         <f>SUM(F4:F10)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G11" s="32">
         <f>SUM(G4:G10)</f>
@@ -5897,7 +5906,7 @@
         <v>7</v>
       </c>
       <c r="K11" s="30">
-        <f t="shared" ref="K4:K11" si="0">$G$11*(1-1/$I$12*J11)</f>
+        <f t="shared" ref="K11" si="1">$G$11*(1-1/$I$12*J11)</f>
         <v>5.999066521458893</v>
       </c>
       <c r="L11" s="30">
@@ -5947,8 +5956,8 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="48" t="s">
         <v>52</v>
       </c>
@@ -6071,7 +6080,7 @@
       <c r="G19" s="28">
         <v>2</v>
       </c>
-      <c r="I19" s="51">
+      <c r="I19" s="45">
         <f>COUNTA(I4:I18)-1</f>
         <v>14</v>
       </c>
@@ -6111,13 +6120,13 @@
     <row r="22" spans="1:13" ht="16.5" customHeight="1"/>
     <row r="23" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="38"/>
@@ -6245,11 +6254,11 @@
       <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
       <c r="F33" s="32">
         <f>SUM(F26:F32)</f>
         <v>2</v>
@@ -6321,8 +6330,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A39" s="52"/>
-      <c r="B39" s="52"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="27" t="s">
         <v>69</v>
       </c>
@@ -6359,8 +6368,8 @@
     <row r="51" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="52" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="53" spans="1:2" ht="18" customHeight="1">
-      <c r="A53" s="52"/>
-      <c r="B53" s="52"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="47"/>
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="55" spans="1:2" ht="15.75" customHeight="1"/>
@@ -6374,8 +6383,8 @@
     <row r="63" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="64" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="65" spans="1:2" ht="18" customHeight="1">
-      <c r="A65" s="52"/>
-      <c r="B65" s="52"/>
+      <c r="A65" s="47"/>
+      <c r="B65" s="47"/>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="67" spans="1:2" ht="15.75" customHeight="1"/>
@@ -6388,8 +6397,8 @@
     <row r="74" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="75" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="76" spans="1:2" ht="18" customHeight="1">
-      <c r="A76" s="52"/>
-      <c r="B76" s="52"/>
+      <c r="A76" s="47"/>
+      <c r="B76" s="47"/>
     </row>
     <row r="77" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="78" spans="1:2" ht="15.75" customHeight="1"/>
@@ -6404,8 +6413,8 @@
     <row r="87" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="88" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="89" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A89" s="52"/>
-      <c r="B89" s="52"/>
+      <c r="A89" s="47"/>
+      <c r="B89" s="47"/>
     </row>
     <row r="90" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="91" spans="1:2" ht="15.75" customHeight="1"/>
@@ -6424,26 +6433,13 @@
     <row r="104" ht="15.75" customHeight="1"/>
     <row r="105" ht="15.75" customHeight="1"/>
     <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="14.45"/>
-    <row r="108" ht="15"/>
-    <row r="109" ht="15"/>
-    <row r="110" ht="15"/>
-    <row r="111" ht="15"/>
-    <row r="112" ht="15"/>
-    <row r="113" ht="15"/>
-    <row r="114" ht="14.45"/>
-    <row r="115" ht="15"/>
-    <row r="116" ht="15"/>
-    <row r="117" ht="15"/>
-    <row r="118" ht="15"/>
-    <row r="119" ht="15"/>
-    <row r="120" ht="15"/>
-    <row r="121" ht="15"/>
-    <row r="122" ht="15"/>
-    <row r="123" ht="15"/>
-    <row r="124" ht="15"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="A76:B76"/>
@@ -6459,11 +6455,6 @@
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="C33:E33"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:J18">
     <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
@@ -6482,67 +6473,67 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="23" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="15" style="23" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" style="23" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="23" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" style="23" customWidth="1"/>
-    <col min="8" max="259" width="14.85546875" style="23" customWidth="1"/>
-    <col min="260" max="260" width="13.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="55.44140625" style="23" customWidth="1"/>
+    <col min="4" max="5" width="17.44140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" style="23" customWidth="1"/>
+    <col min="8" max="259" width="14.88671875" style="23" customWidth="1"/>
+    <col min="260" max="260" width="13.6640625" style="23" customWidth="1"/>
     <col min="261" max="261" width="15" style="23" customWidth="1"/>
-    <col min="262" max="262" width="55.42578125" style="23" customWidth="1"/>
-    <col min="263" max="263" width="33.5703125" style="23" customWidth="1"/>
-    <col min="264" max="264" width="32.7109375" style="23" customWidth="1"/>
-    <col min="265" max="265" width="26.28515625" style="23" customWidth="1"/>
-    <col min="266" max="515" width="14.85546875" style="23" customWidth="1"/>
-    <col min="516" max="516" width="13.7109375" style="23" customWidth="1"/>
+    <col min="262" max="262" width="55.44140625" style="23" customWidth="1"/>
+    <col min="263" max="263" width="33.5546875" style="23" customWidth="1"/>
+    <col min="264" max="264" width="32.6640625" style="23" customWidth="1"/>
+    <col min="265" max="265" width="26.33203125" style="23" customWidth="1"/>
+    <col min="266" max="515" width="14.88671875" style="23" customWidth="1"/>
+    <col min="516" max="516" width="13.6640625" style="23" customWidth="1"/>
     <col min="517" max="517" width="15" style="23" customWidth="1"/>
-    <col min="518" max="518" width="55.42578125" style="23" customWidth="1"/>
-    <col min="519" max="519" width="33.5703125" style="23" customWidth="1"/>
-    <col min="520" max="520" width="32.7109375" style="23" customWidth="1"/>
-    <col min="521" max="521" width="26.28515625" style="23" customWidth="1"/>
-    <col min="522" max="771" width="14.85546875" style="23" customWidth="1"/>
-    <col min="772" max="772" width="13.7109375" style="23" customWidth="1"/>
+    <col min="518" max="518" width="55.44140625" style="23" customWidth="1"/>
+    <col min="519" max="519" width="33.5546875" style="23" customWidth="1"/>
+    <col min="520" max="520" width="32.6640625" style="23" customWidth="1"/>
+    <col min="521" max="521" width="26.33203125" style="23" customWidth="1"/>
+    <col min="522" max="771" width="14.88671875" style="23" customWidth="1"/>
+    <col min="772" max="772" width="13.6640625" style="23" customWidth="1"/>
     <col min="773" max="773" width="15" style="23" customWidth="1"/>
-    <col min="774" max="774" width="55.42578125" style="23" customWidth="1"/>
-    <col min="775" max="775" width="33.5703125" style="23" customWidth="1"/>
-    <col min="776" max="776" width="32.7109375" style="23" customWidth="1"/>
-    <col min="777" max="777" width="26.28515625" style="23" customWidth="1"/>
-    <col min="778" max="1023" width="14.85546875" style="23" customWidth="1"/>
+    <col min="774" max="774" width="55.44140625" style="23" customWidth="1"/>
+    <col min="775" max="775" width="33.5546875" style="23" customWidth="1"/>
+    <col min="776" max="776" width="32.6640625" style="23" customWidth="1"/>
+    <col min="777" max="777" width="26.33203125" style="23" customWidth="1"/>
+    <col min="778" max="1023" width="14.88671875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.45">
-      <c r="K1" s="45" t="s">
+    <row r="1" spans="1:16">
+      <c r="K1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:16" ht="20.25" customHeight="1">
       <c r="A2" s="25"/>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="K2" s="45" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="K2" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45" t="s">
+      <c r="L2" s="46"/>
+      <c r="M2" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="44" t="s">
+      <c r="N2" s="46"/>
+      <c r="O2" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="44"/>
+      <c r="P2" s="53"/>
     </row>
     <row r="3" spans="1:16" ht="18" customHeight="1">
       <c r="C3" s="26" t="s">
@@ -6560,10 +6551,10 @@
       <c r="G3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="45"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="24" t="s">
         <v>37</v>
       </c>
@@ -6880,11 +6871,11 @@
     </row>
     <row r="11" spans="1:16" ht="18" customHeight="1">
       <c r="A11" s="31"/>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="32">
         <f>SUM(F4:F10)</f>
         <v>0</v>
@@ -6929,8 +6920,8 @@
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1"/>
     <row r="14" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="48" t="s">
         <v>52</v>
       </c>
@@ -7019,13 +7010,13 @@
     <row r="20" spans="1:13" ht="16.5" customHeight="1"/>
     <row r="21" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="38"/>
@@ -7185,11 +7176,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
       <c r="F31" s="32">
         <f>SUM(F24:F30)</f>
         <v>0</v>
@@ -7257,8 +7248,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A37" s="52"/>
-      <c r="B37" s="52"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="27" t="s">
         <v>69</v>
       </c>
@@ -7290,13 +7281,13 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="C41" s="26" t="s">
@@ -7429,11 +7420,11 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C49" s="46" t="s">
+      <c r="C49" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
       <c r="F49" s="32">
         <f>SUM(F42:F48)</f>
         <v>17</v>
@@ -7445,8 +7436,8 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="51" spans="1:7" ht="18" customHeight="1">
-      <c r="A51" s="52"/>
-      <c r="B51" s="52"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="48" t="s">
         <v>95</v>
       </c>
@@ -7539,18 +7530,18 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1">
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="53"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C58" s="47" t="s">
+      <c r="C58" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1">
       <c r="C59" s="26" t="s">
@@ -7621,8 +7612,8 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="18" customHeight="1">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
       <c r="C63" s="27" t="s">
         <v>48</v>
       </c>
@@ -7691,11 +7682,11 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="18" customHeight="1">
-      <c r="C67" s="46" t="s">
+      <c r="C67" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D67" s="46"/>
-      <c r="E67" s="46"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
       <c r="F67" s="32">
         <f>SUM(F60:F66)</f>
         <v>40</v>
@@ -7767,8 +7758,8 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="18" customHeight="1">
-      <c r="A73" s="52"/>
-      <c r="B73" s="52"/>
+      <c r="A73" s="47"/>
+      <c r="B73" s="47"/>
       <c r="C73" s="27" t="s">
         <v>69</v>
       </c>
@@ -7802,13 +7793,13 @@
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="76" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C76" s="47" t="s">
+      <c r="C76" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
+      <c r="G76" s="50"/>
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1">
       <c r="C77" s="26" t="s">
@@ -7947,11 +7938,11 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C85" s="46" t="s">
+      <c r="C85" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D85" s="46"/>
-      <c r="E85" s="46"/>
+      <c r="D85" s="51"/>
+      <c r="E85" s="51"/>
       <c r="F85" s="32">
         <f>SUM(F78:F84)</f>
         <v>40</v>
@@ -7962,13 +7953,13 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A86" s="52"/>
-      <c r="B86" s="52"/>
-      <c r="C86" s="53"/>
-      <c r="D86" s="53"/>
-      <c r="E86" s="53"/>
-      <c r="F86" s="53"/>
-      <c r="G86" s="53"/>
+      <c r="A86" s="47"/>
+      <c r="B86" s="47"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="52"/>
+      <c r="F86" s="52"/>
+      <c r="G86" s="52"/>
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1">
       <c r="C87" s="48" t="s">
@@ -8064,13 +8055,13 @@
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="94" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C94" s="47" t="s">
+      <c r="C94" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="D94" s="47"/>
-      <c r="E94" s="47"/>
-      <c r="F94" s="47"/>
-      <c r="G94" s="47"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="50"/>
+      <c r="F94" s="50"/>
+      <c r="G94" s="50"/>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1">
       <c r="C95" s="26" t="s">
@@ -8209,11 +8200,11 @@
       </c>
     </row>
     <row r="103" spans="3:7" ht="15.75" customHeight="1">
-      <c r="C103" s="46" t="s">
+      <c r="C103" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D103" s="46"/>
-      <c r="E103" s="46"/>
+      <c r="D103" s="51"/>
+      <c r="E103" s="51"/>
       <c r="F103" s="32">
         <f>SUM(F96:F102)</f>
         <v>40</v>
@@ -8223,8 +8214,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="3:7" ht="14.45"/>
-    <row r="105" spans="3:7" ht="14.45">
+    <row r="105" spans="3:7" ht="17.399999999999999">
       <c r="C105" s="48" t="s">
         <v>101</v>
       </c>
@@ -8233,7 +8223,7 @@
       <c r="F105" s="48"/>
       <c r="G105" s="48"/>
     </row>
-    <row r="106" spans="3:7" ht="14.45">
+    <row r="106" spans="3:7" ht="18">
       <c r="C106" s="34" t="s">
         <v>31</v>
       </c>
@@ -8250,7 +8240,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="107" spans="3:7" ht="14.45">
+    <row r="107" spans="3:7" ht="15.6">
       <c r="C107" s="27" t="s">
         <v>67</v>
       </c>
@@ -8267,7 +8257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="3:7" ht="14.45">
+    <row r="108" spans="3:7" ht="15.6">
       <c r="C108" s="27" t="s">
         <v>74</v>
       </c>
@@ -8284,7 +8274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="3:7" ht="14.45">
+    <row r="109" spans="3:7" ht="15.6">
       <c r="C109" s="27" t="s">
         <v>69</v>
       </c>
@@ -8301,7 +8291,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="3:7" ht="14.45">
+    <row r="110" spans="3:7" ht="17.399999999999999">
       <c r="C110" s="49" t="s">
         <v>30</v>
       </c>
@@ -8316,17 +8306,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="3:7" ht="14.45"/>
-    <row r="112" spans="3:7" ht="14.45">
-      <c r="C112" s="47" t="s">
+    <row r="112" spans="3:7" ht="18">
+      <c r="C112" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
-      <c r="F112" s="47"/>
-      <c r="G112" s="47"/>
-    </row>
-    <row r="113" spans="3:7" ht="14.45">
+      <c r="D112" s="50"/>
+      <c r="E112" s="50"/>
+      <c r="F112" s="50"/>
+      <c r="G112" s="50"/>
+    </row>
+    <row r="113" spans="3:7" ht="18">
       <c r="C113" s="26" t="s">
         <v>31</v>
       </c>
@@ -8343,7 +8332,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="114" spans="3:7" ht="14.45">
+    <row r="114" spans="3:7" ht="15.6">
       <c r="C114" s="27" t="s">
         <v>67</v>
       </c>
@@ -8360,7 +8349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="3:7" ht="14.45">
+    <row r="115" spans="3:7" ht="15.6">
       <c r="C115" s="27" t="s">
         <v>74</v>
       </c>
@@ -8377,7 +8366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="3:7" ht="14.45">
+    <row r="116" spans="3:7" ht="15.6">
       <c r="C116" s="27" t="s">
         <v>69</v>
       </c>
@@ -8394,7 +8383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="3:7" ht="14.45">
+    <row r="117" spans="3:7" ht="15.6">
       <c r="C117" s="27" t="s">
         <v>48</v>
       </c>
@@ -8411,7 +8400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="3:7" ht="14.45">
+    <row r="118" spans="3:7" ht="15.6">
       <c r="C118" s="27" t="s">
         <v>49</v>
       </c>
@@ -8428,7 +8417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="3:7" ht="14.45">
+    <row r="119" spans="3:7" ht="15.6">
       <c r="C119" s="27" t="s">
         <v>50</v>
       </c>
@@ -8445,7 +8434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="3:7" ht="14.45">
+    <row r="120" spans="3:7" ht="15.6">
       <c r="C120" s="27" t="s">
         <v>51</v>
       </c>
@@ -8462,12 +8451,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="3:7" ht="14.45">
-      <c r="C121" s="46" t="s">
+    <row r="121" spans="3:7" ht="18">
+      <c r="C121" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D121" s="46"/>
-      <c r="E121" s="46"/>
+      <c r="D121" s="51"/>
+      <c r="E121" s="51"/>
       <c r="F121" s="32">
         <f>SUM(F114:F120)</f>
         <v>40</v>
@@ -8479,21 +8468,14 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="C110:E110"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C19:E19"/>
@@ -8510,14 +8492,21 @@
     <mergeCell ref="C57:E57"/>
     <mergeCell ref="C58:G58"/>
     <mergeCell ref="A63:B63"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="C110:E110"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:J11">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
@@ -8536,67 +8525,67 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="23" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="15" style="23" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" style="23" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="23" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" style="23" customWidth="1"/>
-    <col min="8" max="259" width="14.85546875" style="23" customWidth="1"/>
-    <col min="260" max="260" width="13.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="55.44140625" style="23" customWidth="1"/>
+    <col min="4" max="5" width="17.44140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" style="23" customWidth="1"/>
+    <col min="8" max="259" width="14.88671875" style="23" customWidth="1"/>
+    <col min="260" max="260" width="13.6640625" style="23" customWidth="1"/>
     <col min="261" max="261" width="15" style="23" customWidth="1"/>
-    <col min="262" max="262" width="55.42578125" style="23" customWidth="1"/>
-    <col min="263" max="263" width="33.5703125" style="23" customWidth="1"/>
-    <col min="264" max="264" width="32.7109375" style="23" customWidth="1"/>
-    <col min="265" max="265" width="26.28515625" style="23" customWidth="1"/>
-    <col min="266" max="515" width="14.85546875" style="23" customWidth="1"/>
-    <col min="516" max="516" width="13.7109375" style="23" customWidth="1"/>
+    <col min="262" max="262" width="55.44140625" style="23" customWidth="1"/>
+    <col min="263" max="263" width="33.5546875" style="23" customWidth="1"/>
+    <col min="264" max="264" width="32.6640625" style="23" customWidth="1"/>
+    <col min="265" max="265" width="26.33203125" style="23" customWidth="1"/>
+    <col min="266" max="515" width="14.88671875" style="23" customWidth="1"/>
+    <col min="516" max="516" width="13.6640625" style="23" customWidth="1"/>
     <col min="517" max="517" width="15" style="23" customWidth="1"/>
-    <col min="518" max="518" width="55.42578125" style="23" customWidth="1"/>
-    <col min="519" max="519" width="33.5703125" style="23" customWidth="1"/>
-    <col min="520" max="520" width="32.7109375" style="23" customWidth="1"/>
-    <col min="521" max="521" width="26.28515625" style="23" customWidth="1"/>
-    <col min="522" max="771" width="14.85546875" style="23" customWidth="1"/>
-    <col min="772" max="772" width="13.7109375" style="23" customWidth="1"/>
+    <col min="518" max="518" width="55.44140625" style="23" customWidth="1"/>
+    <col min="519" max="519" width="33.5546875" style="23" customWidth="1"/>
+    <col min="520" max="520" width="32.6640625" style="23" customWidth="1"/>
+    <col min="521" max="521" width="26.33203125" style="23" customWidth="1"/>
+    <col min="522" max="771" width="14.88671875" style="23" customWidth="1"/>
+    <col min="772" max="772" width="13.6640625" style="23" customWidth="1"/>
     <col min="773" max="773" width="15" style="23" customWidth="1"/>
-    <col min="774" max="774" width="55.42578125" style="23" customWidth="1"/>
-    <col min="775" max="775" width="33.5703125" style="23" customWidth="1"/>
-    <col min="776" max="776" width="32.7109375" style="23" customWidth="1"/>
-    <col min="777" max="777" width="26.28515625" style="23" customWidth="1"/>
-    <col min="778" max="1023" width="14.85546875" style="23" customWidth="1"/>
+    <col min="774" max="774" width="55.44140625" style="23" customWidth="1"/>
+    <col min="775" max="775" width="33.5546875" style="23" customWidth="1"/>
+    <col min="776" max="776" width="32.6640625" style="23" customWidth="1"/>
+    <col min="777" max="777" width="26.33203125" style="23" customWidth="1"/>
+    <col min="778" max="1023" width="14.88671875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.45">
-      <c r="K1" s="45" t="s">
+    <row r="1" spans="1:16">
+      <c r="K1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:16" ht="20.25" customHeight="1">
       <c r="A2" s="25"/>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="K2" s="45" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="K2" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45" t="s">
+      <c r="L2" s="46"/>
+      <c r="M2" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="44" t="s">
+      <c r="N2" s="46"/>
+      <c r="O2" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="44"/>
+      <c r="P2" s="53"/>
     </row>
     <row r="3" spans="1:16" ht="18" customHeight="1">
       <c r="C3" s="26" t="s">
@@ -8614,10 +8603,10 @@
       <c r="G3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="45"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="24" t="s">
         <v>37</v>
       </c>
@@ -8948,11 +8937,11 @@
     </row>
     <row r="11" spans="1:16" ht="18" customHeight="1">
       <c r="A11" s="31"/>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="32">
         <f>SUM(F4:F10)</f>
         <v>40</v>
@@ -8997,8 +8986,8 @@
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1"/>
     <row r="14" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="48" t="s">
         <v>52</v>
       </c>
@@ -9093,13 +9082,13 @@
     <row r="20" spans="1:13" ht="16.5" customHeight="1"/>
     <row r="21" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="38"/>
@@ -9273,11 +9262,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
       <c r="F31" s="32">
         <f>SUM(F24:F30)</f>
         <v>40</v>
@@ -9349,8 +9338,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A37" s="52"/>
-      <c r="B37" s="52"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="27" t="s">
         <v>69</v>
       </c>
@@ -9384,13 +9373,13 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="C41" s="26" t="s">
@@ -9529,11 +9518,11 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C49" s="46" t="s">
+      <c r="C49" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
       <c r="F49" s="32">
         <f>SUM(F42:F48)</f>
         <v>40</v>
@@ -9545,8 +9534,8 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="51" spans="1:7" ht="18" customHeight="1">
-      <c r="A51" s="52"/>
-      <c r="B51" s="52"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="48" t="s">
         <v>95</v>
       </c>
@@ -9639,18 +9628,18 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1">
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="53"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C58" s="47" t="s">
+      <c r="C58" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1">
       <c r="C59" s="26" t="s">
@@ -9721,8 +9710,8 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="18" customHeight="1">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
       <c r="C63" s="27" t="s">
         <v>48</v>
       </c>
@@ -9791,11 +9780,11 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="18" customHeight="1">
-      <c r="C67" s="46" t="s">
+      <c r="C67" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D67" s="46"/>
-      <c r="E67" s="46"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
       <c r="F67" s="32">
         <f>SUM(F60:F66)</f>
         <v>40</v>
@@ -9867,8 +9856,8 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="18" customHeight="1">
-      <c r="A73" s="52"/>
-      <c r="B73" s="52"/>
+      <c r="A73" s="47"/>
+      <c r="B73" s="47"/>
       <c r="C73" s="27" t="s">
         <v>69</v>
       </c>
@@ -9902,13 +9891,13 @@
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="76" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C76" s="47" t="s">
+      <c r="C76" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
+      <c r="G76" s="50"/>
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1">
       <c r="C77" s="26" t="s">
@@ -10047,11 +10036,11 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C85" s="46" t="s">
+      <c r="C85" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D85" s="46"/>
-      <c r="E85" s="46"/>
+      <c r="D85" s="51"/>
+      <c r="E85" s="51"/>
       <c r="F85" s="32">
         <f>SUM(F78:F84)</f>
         <v>40</v>
@@ -10062,13 +10051,13 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A86" s="52"/>
-      <c r="B86" s="52"/>
-      <c r="C86" s="53"/>
-      <c r="D86" s="53"/>
-      <c r="E86" s="53"/>
-      <c r="F86" s="53"/>
-      <c r="G86" s="53"/>
+      <c r="A86" s="47"/>
+      <c r="B86" s="47"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="52"/>
+      <c r="F86" s="52"/>
+      <c r="G86" s="52"/>
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1">
       <c r="C87" s="48" t="s">
@@ -10164,13 +10153,13 @@
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="94" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C94" s="47" t="s">
+      <c r="C94" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="D94" s="47"/>
-      <c r="E94" s="47"/>
-      <c r="F94" s="47"/>
-      <c r="G94" s="47"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="50"/>
+      <c r="F94" s="50"/>
+      <c r="G94" s="50"/>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1">
       <c r="C95" s="26" t="s">
@@ -10309,11 +10298,11 @@
       </c>
     </row>
     <row r="103" spans="3:7" ht="15.75" customHeight="1">
-      <c r="C103" s="46" t="s">
+      <c r="C103" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D103" s="46"/>
-      <c r="E103" s="46"/>
+      <c r="D103" s="51"/>
+      <c r="E103" s="51"/>
       <c r="F103" s="32">
         <f>SUM(F96:F102)</f>
         <v>40</v>
@@ -10323,8 +10312,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="3:7" ht="14.45"/>
-    <row r="105" spans="3:7" ht="14.45">
+    <row r="105" spans="3:7" ht="17.399999999999999">
       <c r="C105" s="48" t="s">
         <v>101</v>
       </c>
@@ -10333,7 +10321,7 @@
       <c r="F105" s="48"/>
       <c r="G105" s="48"/>
     </row>
-    <row r="106" spans="3:7" ht="14.45">
+    <row r="106" spans="3:7" ht="18">
       <c r="C106" s="34" t="s">
         <v>31</v>
       </c>
@@ -10350,7 +10338,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="107" spans="3:7" ht="14.45">
+    <row r="107" spans="3:7" ht="15.6">
       <c r="C107" s="27" t="s">
         <v>67</v>
       </c>
@@ -10365,7 +10353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="3:7" ht="14.45">
+    <row r="108" spans="3:7" ht="15.6">
       <c r="C108" s="27" t="s">
         <v>74</v>
       </c>
@@ -10380,7 +10368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="3:7" ht="14.45">
+    <row r="109" spans="3:7" ht="15.6">
       <c r="C109" s="27" t="s">
         <v>69</v>
       </c>
@@ -10395,7 +10383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="3:7" ht="14.45">
+    <row r="110" spans="3:7" ht="17.399999999999999">
       <c r="C110" s="49" t="s">
         <v>30</v>
       </c>
@@ -10410,17 +10398,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="3:7" ht="14.45"/>
-    <row r="112" spans="3:7" ht="14.45">
-      <c r="C112" s="47" t="s">
+    <row r="112" spans="3:7" ht="18">
+      <c r="C112" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
-      <c r="F112" s="47"/>
-      <c r="G112" s="47"/>
-    </row>
-    <row r="113" spans="3:7" ht="14.45">
+      <c r="D112" s="50"/>
+      <c r="E112" s="50"/>
+      <c r="F112" s="50"/>
+      <c r="G112" s="50"/>
+    </row>
+    <row r="113" spans="3:7" ht="18">
       <c r="C113" s="26" t="s">
         <v>31</v>
       </c>
@@ -10437,7 +10424,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="114" spans="3:7" ht="14.45">
+    <row r="114" spans="3:7" ht="15.6">
       <c r="C114" s="27" t="s">
         <v>67</v>
       </c>
@@ -10452,7 +10439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="3:7" ht="14.45">
+    <row r="115" spans="3:7" ht="15.6">
       <c r="C115" s="27" t="s">
         <v>74</v>
       </c>
@@ -10467,7 +10454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="3:7" ht="14.45">
+    <row r="116" spans="3:7" ht="15.6">
       <c r="C116" s="27" t="s">
         <v>69</v>
       </c>
@@ -10482,7 +10469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="3:7" ht="14.45">
+    <row r="117" spans="3:7" ht="15.6">
       <c r="C117" s="27" t="s">
         <v>48</v>
       </c>
@@ -10497,7 +10484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="3:7" ht="14.45">
+    <row r="118" spans="3:7" ht="15.6">
       <c r="C118" s="27" t="s">
         <v>49</v>
       </c>
@@ -10512,7 +10499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="3:7" ht="14.45">
+    <row r="119" spans="3:7" ht="15.6">
       <c r="C119" s="27" t="s">
         <v>50</v>
       </c>
@@ -10527,7 +10514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="3:7" ht="14.45">
+    <row r="120" spans="3:7" ht="15.6">
       <c r="C120" s="27" t="s">
         <v>51</v>
       </c>
@@ -10542,12 +10529,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="3:7" ht="14.45">
-      <c r="C121" s="46" t="s">
+    <row r="121" spans="3:7" ht="18">
+      <c r="C121" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D121" s="46"/>
-      <c r="E121" s="46"/>
+      <c r="D121" s="51"/>
+      <c r="E121" s="51"/>
       <c r="F121" s="32">
         <f>SUM(F114:F120)</f>
         <v>0</v>
@@ -10559,21 +10546,14 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="C110:E110"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C19:E19"/>
@@ -10590,14 +10570,21 @@
     <mergeCell ref="C57:E57"/>
     <mergeCell ref="C58:G58"/>
     <mergeCell ref="A63:B63"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="C110:E110"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:J11">
     <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
@@ -10616,67 +10603,67 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="23" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="15" style="23" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" style="23" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="23" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" style="23" customWidth="1"/>
-    <col min="8" max="259" width="14.85546875" style="23" customWidth="1"/>
-    <col min="260" max="260" width="13.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="55.44140625" style="23" customWidth="1"/>
+    <col min="4" max="5" width="17.44140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" style="23" customWidth="1"/>
+    <col min="8" max="259" width="14.88671875" style="23" customWidth="1"/>
+    <col min="260" max="260" width="13.6640625" style="23" customWidth="1"/>
     <col min="261" max="261" width="15" style="23" customWidth="1"/>
-    <col min="262" max="262" width="55.42578125" style="23" customWidth="1"/>
-    <col min="263" max="263" width="33.5703125" style="23" customWidth="1"/>
-    <col min="264" max="264" width="32.7109375" style="23" customWidth="1"/>
-    <col min="265" max="265" width="26.28515625" style="23" customWidth="1"/>
-    <col min="266" max="515" width="14.85546875" style="23" customWidth="1"/>
-    <col min="516" max="516" width="13.7109375" style="23" customWidth="1"/>
+    <col min="262" max="262" width="55.44140625" style="23" customWidth="1"/>
+    <col min="263" max="263" width="33.5546875" style="23" customWidth="1"/>
+    <col min="264" max="264" width="32.6640625" style="23" customWidth="1"/>
+    <col min="265" max="265" width="26.33203125" style="23" customWidth="1"/>
+    <col min="266" max="515" width="14.88671875" style="23" customWidth="1"/>
+    <col min="516" max="516" width="13.6640625" style="23" customWidth="1"/>
     <col min="517" max="517" width="15" style="23" customWidth="1"/>
-    <col min="518" max="518" width="55.42578125" style="23" customWidth="1"/>
-    <col min="519" max="519" width="33.5703125" style="23" customWidth="1"/>
-    <col min="520" max="520" width="32.7109375" style="23" customWidth="1"/>
-    <col min="521" max="521" width="26.28515625" style="23" customWidth="1"/>
-    <col min="522" max="771" width="14.85546875" style="23" customWidth="1"/>
-    <col min="772" max="772" width="13.7109375" style="23" customWidth="1"/>
+    <col min="518" max="518" width="55.44140625" style="23" customWidth="1"/>
+    <col min="519" max="519" width="33.5546875" style="23" customWidth="1"/>
+    <col min="520" max="520" width="32.6640625" style="23" customWidth="1"/>
+    <col min="521" max="521" width="26.33203125" style="23" customWidth="1"/>
+    <col min="522" max="771" width="14.88671875" style="23" customWidth="1"/>
+    <col min="772" max="772" width="13.6640625" style="23" customWidth="1"/>
     <col min="773" max="773" width="15" style="23" customWidth="1"/>
-    <col min="774" max="774" width="55.42578125" style="23" customWidth="1"/>
-    <col min="775" max="775" width="33.5703125" style="23" customWidth="1"/>
-    <col min="776" max="776" width="32.7109375" style="23" customWidth="1"/>
-    <col min="777" max="777" width="26.28515625" style="23" customWidth="1"/>
-    <col min="778" max="1023" width="14.85546875" style="23" customWidth="1"/>
+    <col min="774" max="774" width="55.44140625" style="23" customWidth="1"/>
+    <col min="775" max="775" width="33.5546875" style="23" customWidth="1"/>
+    <col min="776" max="776" width="32.6640625" style="23" customWidth="1"/>
+    <col min="777" max="777" width="26.33203125" style="23" customWidth="1"/>
+    <col min="778" max="1023" width="14.88671875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.45">
-      <c r="K1" s="45" t="s">
+    <row r="1" spans="1:16">
+      <c r="K1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:16" ht="20.25" customHeight="1">
       <c r="A2" s="25"/>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="K2" s="45" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="K2" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45" t="s">
+      <c r="L2" s="46"/>
+      <c r="M2" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="44" t="s">
+      <c r="N2" s="46"/>
+      <c r="O2" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="44"/>
+      <c r="P2" s="53"/>
     </row>
     <row r="3" spans="1:16" ht="18" customHeight="1">
       <c r="C3" s="26" t="s">
@@ -10694,10 +10681,10 @@
       <c r="G3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="45"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="24" t="s">
         <v>37</v>
       </c>
@@ -11014,11 +11001,11 @@
     </row>
     <row r="11" spans="1:16" ht="18" customHeight="1">
       <c r="A11" s="31"/>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="32">
         <f>SUM(F4:F10)</f>
         <v>0</v>
@@ -11063,8 +11050,8 @@
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1"/>
     <row r="14" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="48" t="s">
         <v>52</v>
       </c>
@@ -11153,13 +11140,13 @@
     <row r="20" spans="1:13" ht="16.5" customHeight="1"/>
     <row r="21" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="38"/>
@@ -11319,11 +11306,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
       <c r="F31" s="32">
         <f>SUM(F24:F30)</f>
         <v>0</v>
@@ -11395,8 +11382,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A37" s="52"/>
-      <c r="B37" s="52"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="27" t="s">
         <v>69</v>
       </c>
@@ -11430,13 +11417,13 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="C41" s="26" t="s">
@@ -11575,11 +11562,11 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C49" s="46" t="s">
+      <c r="C49" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
       <c r="F49" s="32">
         <f>SUM(F42:F48)</f>
         <v>40</v>
@@ -11591,8 +11578,8 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="51" spans="1:7" ht="18" customHeight="1">
-      <c r="A51" s="52"/>
-      <c r="B51" s="52"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="48" t="s">
         <v>95</v>
       </c>
@@ -11685,18 +11672,18 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1">
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="53"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C58" s="47" t="s">
+      <c r="C58" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1">
       <c r="C59" s="26" t="s">
@@ -11767,8 +11754,8 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="18" customHeight="1">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
       <c r="C63" s="27" t="s">
         <v>48</v>
       </c>
@@ -11837,11 +11824,11 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="18" customHeight="1">
-      <c r="C67" s="46" t="s">
+      <c r="C67" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D67" s="46"/>
-      <c r="E67" s="46"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
       <c r="F67" s="32">
         <f>SUM(F60:F66)</f>
         <v>40</v>
@@ -11913,8 +11900,8 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="18" customHeight="1">
-      <c r="A73" s="52"/>
-      <c r="B73" s="52"/>
+      <c r="A73" s="47"/>
+      <c r="B73" s="47"/>
       <c r="C73" s="27" t="s">
         <v>69</v>
       </c>
@@ -11948,13 +11935,13 @@
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="76" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C76" s="47" t="s">
+      <c r="C76" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
+      <c r="G76" s="50"/>
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1">
       <c r="C77" s="26" t="s">
@@ -12093,11 +12080,11 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C85" s="46" t="s">
+      <c r="C85" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D85" s="46"/>
-      <c r="E85" s="46"/>
+      <c r="D85" s="51"/>
+      <c r="E85" s="51"/>
       <c r="F85" s="32">
         <f>SUM(F78:F84)</f>
         <v>40</v>
@@ -12108,13 +12095,13 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A86" s="52"/>
-      <c r="B86" s="52"/>
-      <c r="C86" s="53"/>
-      <c r="D86" s="53"/>
-      <c r="E86" s="53"/>
-      <c r="F86" s="53"/>
-      <c r="G86" s="53"/>
+      <c r="A86" s="47"/>
+      <c r="B86" s="47"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="52"/>
+      <c r="F86" s="52"/>
+      <c r="G86" s="52"/>
     </row>
     <row r="87" spans="1:7" ht="15.75" customHeight="1">
       <c r="C87" s="48" t="s">
@@ -12210,13 +12197,13 @@
     </row>
     <row r="93" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="94" spans="1:7" ht="15.75" customHeight="1">
-      <c r="C94" s="47" t="s">
+      <c r="C94" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="D94" s="47"/>
-      <c r="E94" s="47"/>
-      <c r="F94" s="47"/>
-      <c r="G94" s="47"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="50"/>
+      <c r="F94" s="50"/>
+      <c r="G94" s="50"/>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1">
       <c r="C95" s="26" t="s">
@@ -12355,11 +12342,11 @@
       </c>
     </row>
     <row r="103" spans="3:7" ht="15.75" customHeight="1">
-      <c r="C103" s="46" t="s">
+      <c r="C103" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D103" s="46"/>
-      <c r="E103" s="46"/>
+      <c r="D103" s="51"/>
+      <c r="E103" s="51"/>
       <c r="F103" s="32">
         <f>SUM(F96:F102)</f>
         <v>40</v>
@@ -12369,8 +12356,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="3:7" ht="14.45"/>
-    <row r="105" spans="3:7" ht="14.45">
+    <row r="105" spans="3:7" ht="17.399999999999999">
       <c r="C105" s="48" t="s">
         <v>101</v>
       </c>
@@ -12379,7 +12365,7 @@
       <c r="F105" s="48"/>
       <c r="G105" s="48"/>
     </row>
-    <row r="106" spans="3:7" ht="14.45">
+    <row r="106" spans="3:7" ht="18">
       <c r="C106" s="34" t="s">
         <v>31</v>
       </c>
@@ -12396,7 +12382,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="107" spans="3:7" ht="14.45">
+    <row r="107" spans="3:7" ht="15.6">
       <c r="C107" s="27" t="s">
         <v>67</v>
       </c>
@@ -12413,7 +12399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="3:7" ht="14.45">
+    <row r="108" spans="3:7" ht="15.6">
       <c r="C108" s="27" t="s">
         <v>74</v>
       </c>
@@ -12430,7 +12416,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="3:7" ht="14.45">
+    <row r="109" spans="3:7" ht="15.6">
       <c r="C109" s="27" t="s">
         <v>69</v>
       </c>
@@ -12447,7 +12433,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="3:7" ht="14.45">
+    <row r="110" spans="3:7" ht="17.399999999999999">
       <c r="C110" s="49" t="s">
         <v>30</v>
       </c>
@@ -12462,17 +12448,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="3:7" ht="14.45"/>
-    <row r="112" spans="3:7" ht="14.45">
-      <c r="C112" s="47" t="s">
+    <row r="112" spans="3:7" ht="18">
+      <c r="C112" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
-      <c r="F112" s="47"/>
-      <c r="G112" s="47"/>
-    </row>
-    <row r="113" spans="3:7" ht="14.45">
+      <c r="D112" s="50"/>
+      <c r="E112" s="50"/>
+      <c r="F112" s="50"/>
+      <c r="G112" s="50"/>
+    </row>
+    <row r="113" spans="3:7" ht="18">
       <c r="C113" s="26" t="s">
         <v>31</v>
       </c>
@@ -12489,7 +12474,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="114" spans="3:7" ht="14.45">
+    <row r="114" spans="3:7" ht="15.6">
       <c r="C114" s="27" t="s">
         <v>67</v>
       </c>
@@ -12506,7 +12491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="3:7" ht="14.45">
+    <row r="115" spans="3:7" ht="15.6">
       <c r="C115" s="27" t="s">
         <v>74</v>
       </c>
@@ -12523,7 +12508,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="3:7" ht="14.45">
+    <row r="116" spans="3:7" ht="15.6">
       <c r="C116" s="27" t="s">
         <v>69</v>
       </c>
@@ -12540,7 +12525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="3:7" ht="14.45">
+    <row r="117" spans="3:7" ht="15.6">
       <c r="C117" s="27" t="s">
         <v>48</v>
       </c>
@@ -12557,7 +12542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="3:7" ht="14.45">
+    <row r="118" spans="3:7" ht="15.6">
       <c r="C118" s="27" t="s">
         <v>49</v>
       </c>
@@ -12574,7 +12559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="3:7" ht="14.45">
+    <row r="119" spans="3:7" ht="15.6">
       <c r="C119" s="27" t="s">
         <v>50</v>
       </c>
@@ -12591,7 +12576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="3:7" ht="14.45">
+    <row r="120" spans="3:7" ht="15.6">
       <c r="C120" s="27" t="s">
         <v>51</v>
       </c>
@@ -12608,12 +12593,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="3:7" ht="14.45">
-      <c r="C121" s="46" t="s">
+    <row r="121" spans="3:7" ht="18">
+      <c r="C121" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D121" s="46"/>
-      <c r="E121" s="46"/>
+      <c r="D121" s="51"/>
+      <c r="E121" s="51"/>
       <c r="F121" s="32">
         <f>SUM(F114:F120)</f>
         <v>40</v>
@@ -12625,21 +12610,14 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C105:G105"/>
-    <mergeCell ref="C110:E110"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C19:E19"/>
@@ -12656,14 +12634,21 @@
     <mergeCell ref="C57:E57"/>
     <mergeCell ref="C58:G58"/>
     <mergeCell ref="A63:B63"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="C110:E110"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:J11">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
@@ -12815,12 +12800,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -12829,14 +12808,43 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B90CA24E-A780-466D-A56D-2169B3CA1B5D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B90CA24E-A780-466D-A56D-2169B3CA1B5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1067841d-428a-434c-8d98-4cc88b65cff9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AA356FC-64FE-4673-8E51-FB0D8650E9C9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82FDAA87-3D8E-46E8-8A31-FFB51E86F013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82FDAA87-3D8E-46E8-8A31-FFB51E86F013}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AA356FC-64FE-4673-8E51-FB0D8650E9C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>